<commit_message>
fix the desc of summon draconic spirit
</commit_message>
<xml_diff>
--- a/dndspells.xlsx
+++ b/dndspells.xlsx
@@ -5,36 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultad\rol\js\Cartitas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Gonza\3 - Proyectos\1.2 - portfolio nuevo\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD6B5F9-856F-40E3-9045-1F62DFD0B828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9369A53-ECF9-4B8E-84FD-9FAC39E728E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spells" sheetId="1" r:id="rId1"/>
     <sheet name="Summons" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3892" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3893" uniqueCount="1194">
   <si>
     <t>Name</t>
   </si>
@@ -4716,6 +4703,10 @@
   <si>
     <t>You weave together threads of shadow to create a sword of solidified gloom in your hand. This magic sword lasts until the spell ends. It counts as a simple melee weapon with which you are proficient. It deals 2d8 psychic damage on a hit and has the finesse, light, and thrown properties (range 20/60). In addition, when you use the sword to attack a target that is in dim light or darkness, you make the attack roll with advantage. If you drop the weapon or throw it, it dissipates at the end of the turn. Thereafter, while the spell persists, you can use a bonus action to cause the sword to reappear in your hand.
 When you cast this spell using a (3-4)th spell slot, the damage is 3d8 - (5-6)th spell slot, the damage is 4d8 - 7th level or higher, the damage is 5d8.</t>
+  </si>
+  <si>
+    <t>You call forth a draconic spirit. It manifests in an unoccupied space that you can see within range. This corporeal form uses the Draconic Spirit stat block. When you cast this spell, choose a family of dragon: chromatic, gem, or metallic. The creature resembles a dragon of the chosen family, which determines certain traits in its stat block. The creature disappears when it drops to 0 hit points or when the spell ends.
+The creature is an ally to you and your companions. In combat, the creature shares your initiative count, but it takes its turn immediately after yours. It obeys your verbal commands (no action required by you). If you don’t issue any, it takes the Dodge action and uses its move to avoid danger.</t>
   </si>
 </sst>
 </file>
@@ -5036,8 +5027,8 @@
   </sheetPr>
   <dimension ref="A1:N1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="G194" sqref="G194"/>
+    <sheetView tabSelected="1" topLeftCell="A504" workbookViewId="0">
+      <selection activeCell="H388" sqref="H388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17767,7 +17758,9 @@
       <c r="G387" s="3" t="s">
         <v>1131</v>
       </c>
-      <c r="H387" s="3"/>
+      <c r="H387" s="9" t="s">
+        <v>1193</v>
+      </c>
       <c r="I387" s="3"/>
       <c r="J387" s="2"/>
       <c r="K387" s="2"/>

</xml_diff>